<commit_message>
Ajout coordonnées supp. pour me joindre.
Dingueling!
</commit_message>
<xml_diff>
--- a/Adressbook.xlsx
+++ b/Adressbook.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="5205"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Francis Valois</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>EMARS2</t>
+  </si>
+  <si>
+    <t>(maison) 418-847-7722</t>
+  </si>
+  <si>
+    <t>plbuhler01@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -168,9 +174,10 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -184,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -470,21 +477,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -494,11 +503,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -508,11 +517,11 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -522,11 +531,11 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -536,11 +545,11 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -550,25 +559,31 @@
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -578,11 +593,11 @@
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -592,31 +607,32 @@
       <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" display="tel:418-271-7831"/>
+    <hyperlink ref="E8" r:id="rId1" display="tel:418-271-7831"/>
     <hyperlink ref="C8" r:id="rId2" display="mailto:imanemouhtij@hotmail.com"/>
-    <hyperlink ref="D7" r:id="rId3" display="tel:418-931-8720"/>
+    <hyperlink ref="E7" r:id="rId3" display="tel:418-931-8720"/>
     <hyperlink ref="C7" r:id="rId4" display="mailto:emile.arsenault.1@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId5" display="tel:581-777-0237"/>
-    <hyperlink ref="C6" r:id="rId6" display="mailto:pierre-luc.buhler.1@ulaval.ca"/>
-    <hyperlink ref="D5" r:id="rId7" display="tel:418-563-9854"/>
+    <hyperlink ref="E6" r:id="rId5" display="tel:581-777-0237"/>
+    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7" display="tel:418-563-9854"/>
     <hyperlink ref="C5" r:id="rId8" display="mailto:philippe.bourdages@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId9" display="tel:418-455-1155"/>
+    <hyperlink ref="E4" r:id="rId9" display="tel:418-455-1155"/>
     <hyperlink ref="C4" r:id="rId10" display="mailto:diane.fournier.3@ulaval.ca"/>
-    <hyperlink ref="D3" r:id="rId11" display="tel:418-456-3734"/>
+    <hyperlink ref="E3" r:id="rId11" display="tel:418-456-3734"/>
     <hyperlink ref="C3" r:id="rId12" display="mailto:g.oliviersylvain@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId13" display="tel:%28581%29 997-6656"/>
+    <hyperlink ref="E2" r:id="rId13" display="tel:%28581%29 997-6656"/>
     <hyperlink ref="C2" r:id="rId14" display="mailto:danthib76@gmail.com"/>
-    <hyperlink ref="D1" r:id="rId15" display="tel:581-307-0691"/>
+    <hyperlink ref="E1" r:id="rId15" display="tel:581-307-0691"/>
     <hyperlink ref="C1" r:id="rId16" display="mailto:francis.valois1@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -626,7 +642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -638,7 +654,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modifs AdressBook + DPF_alternatif.xls
</commit_message>
<xml_diff>
--- a/Adressbook.xlsx
+++ b/Adressbook.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="5205"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -63,9 +63,6 @@
     <t>diane.fournier.3@ulaval.ca</t>
   </si>
   <si>
-    <t>418-455-1155</t>
-  </si>
-  <si>
     <t>Philippe Bourdages</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>plbuhler01@gmail.com</t>
+  </si>
+  <si>
+    <t>418-455-1115</t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -480,10 +480,10 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -546,69 +546,69 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -642,7 +642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -654,7 +654,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correction numero telephone Philippe.
</commit_message>
<xml_diff>
--- a/Adressbook.xlsx
+++ b/Adressbook.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="5205"/>
@@ -72,9 +72,6 @@
     <t>philippe.bourdages@gmail.com</t>
   </si>
   <si>
-    <t>418-563-9854</t>
-  </si>
-  <si>
     <t>Pierre-Luc Buhler</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>418-455-1115</t>
+  </si>
+  <si>
+    <t>418-563-8564</t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -483,7 +483,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -546,7 +546,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -560,55 +560,55 @@
         <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -642,7 +642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -654,7 +654,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MAJ de la logistique
</commit_message>
<xml_diff>
--- a/Adressbook.xlsx
+++ b/Adressbook.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="5205"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Francis Valois</t>
   </si>
@@ -91,18 +91,6 @@
   </si>
   <si>
     <t>418-931-8720</t>
-  </si>
-  <si>
-    <t>imane Mouhtij</t>
-  </si>
-  <si>
-    <t>imanemouhtij@hotmail.com</t>
-  </si>
-  <si>
-    <t>418-271-7831</t>
-  </si>
-  <si>
-    <t>IMMOU4</t>
   </si>
   <si>
     <t>EMARS2</t>
@@ -177,7 +165,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,7 +179,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -477,13 +465,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -546,7 +534,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -560,7 +548,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -571,7 +559,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
@@ -580,7 +568,7 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -588,51 +576,35 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" display="tel:418-271-7831"/>
-    <hyperlink ref="C8" r:id="rId2" display="mailto:imanemouhtij@hotmail.com"/>
-    <hyperlink ref="E7" r:id="rId3" display="tel:418-931-8720"/>
-    <hyperlink ref="C7" r:id="rId4" display="mailto:emile.arsenault.1@gmail.com"/>
-    <hyperlink ref="E6" r:id="rId5" display="tel:581-777-0237"/>
-    <hyperlink ref="D6" r:id="rId6"/>
-    <hyperlink ref="E5" r:id="rId7" display="tel:418-563-9854"/>
-    <hyperlink ref="C5" r:id="rId8" display="mailto:philippe.bourdages@gmail.com"/>
-    <hyperlink ref="E4" r:id="rId9" display="tel:418-455-1155"/>
-    <hyperlink ref="C4" r:id="rId10" display="mailto:diane.fournier.3@ulaval.ca"/>
-    <hyperlink ref="E3" r:id="rId11" display="tel:418-456-3734"/>
-    <hyperlink ref="C3" r:id="rId12" display="mailto:g.oliviersylvain@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId13" display="tel:%28581%29 997-6656"/>
-    <hyperlink ref="C2" r:id="rId14" display="mailto:danthib76@gmail.com"/>
-    <hyperlink ref="E1" r:id="rId15" display="tel:581-307-0691"/>
-    <hyperlink ref="C1" r:id="rId16" display="mailto:francis.valois1@gmail.com"/>
-    <hyperlink ref="C6" r:id="rId17"/>
+    <hyperlink ref="E7" r:id="rId1" display="tel:418-931-8720"/>
+    <hyperlink ref="C7" r:id="rId2" display="mailto:emile.arsenault.1@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId3" display="tel:581-777-0237"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5" display="tel:418-563-9854"/>
+    <hyperlink ref="C5" r:id="rId6" display="mailto:philippe.bourdages@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId7" display="tel:418-455-1155"/>
+    <hyperlink ref="C4" r:id="rId8" display="mailto:diane.fournier.3@ulaval.ca"/>
+    <hyperlink ref="E3" r:id="rId9" display="tel:418-456-3734"/>
+    <hyperlink ref="C3" r:id="rId10" display="mailto:g.oliviersylvain@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId11" display="tel:%28581%29 997-6656"/>
+    <hyperlink ref="C2" r:id="rId12" display="mailto:danthib76@gmail.com"/>
+    <hyperlink ref="E1" r:id="rId13" display="tel:581-307-0691"/>
+    <hyperlink ref="C1" r:id="rId14" display="mailto:francis.valois1@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -642,7 +614,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -654,7 +626,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>